<commit_message>
suhao update ipo,delist, financesheet
</commit_message>
<xml_diff>
--- a/ipo_delist_within5y_1974_2024_2.xlsx
+++ b/ipo_delist_within5y_1974_2024_2.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G123"/>
+  <dimension ref="A1:G120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -530,23 +530,23 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>68152</v>
+        <v>69091</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>TURNER EQUITY INVESTORS INC</t>
+          <t>ST JOE GOLD CORP</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>TEQ</t>
+          <t>SJG</t>
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>31247</v>
+        <v>31442</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>32498</v>
+        <v>32154</v>
       </c>
       <c r="F4" t="n">
         <v>2</v>
@@ -557,23 +557,23 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>69091</v>
+        <v>69454</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ST JOE GOLD CORP</t>
+          <t>GUILD MORTGAGE INVESTMENTS</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>SJG</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="D5" s="2" t="n">
-        <v>31442</v>
+        <v>31587</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>32154</v>
+        <v>32323</v>
       </c>
       <c r="F5" t="n">
         <v>2</v>
@@ -584,23 +584,23 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>69454</v>
+        <v>70666</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>GUILD MORTGAGE INVESTMENTS</t>
+          <t>GRUEN MARKETING CORP</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>GMC</t>
         </is>
       </c>
       <c r="D6" s="2" t="n">
-        <v>31587</v>
+        <v>31702</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>32323</v>
+        <v>32482</v>
       </c>
       <c r="F6" t="n">
         <v>2</v>
@@ -611,77 +611,77 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>70666</v>
+        <v>70586</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>GRUEN MARKETING CORP</t>
+          <t>EMPIRE OF AMERICA FSB</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>GMC</t>
+          <t>EOA</t>
         </is>
       </c>
       <c r="D7" s="2" t="n">
-        <v>31702</v>
+        <v>31742</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>32482</v>
+        <v>32917</v>
       </c>
       <c r="F7" t="n">
         <v>2</v>
       </c>
       <c r="G7" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>70586</v>
+        <v>70711</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>EMPIRE OF AMERICA FSB</t>
+          <t>HONEYBEE INC</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>EOA</t>
+          <t>HBE</t>
         </is>
       </c>
       <c r="D8" s="2" t="n">
-        <v>31742</v>
+        <v>31765</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>32917</v>
+        <v>32377</v>
       </c>
       <c r="F8" t="n">
         <v>2</v>
       </c>
       <c r="G8" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>70711</v>
+        <v>30082</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>HONEYBEE INC</t>
+          <t>MATRIX CORP-N J</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>HBE</t>
+          <t>MAX</t>
         </is>
       </c>
       <c r="D9" s="2" t="n">
-        <v>31765</v>
+        <v>31778</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>32377</v>
+        <v>32461</v>
       </c>
       <c r="F9" t="n">
         <v>2</v>
@@ -692,50 +692,50 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>30082</v>
+        <v>67280</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>MATRIX CORP-N J</t>
+          <t>CONSOLIDATED COS</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>MAX</t>
+          <t>JAC</t>
         </is>
       </c>
       <c r="D10" s="2" t="n">
         <v>31778</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>32461</v>
+        <v>32574</v>
       </c>
       <c r="F10" t="n">
         <v>2</v>
       </c>
       <c r="G10" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>67280</v>
+        <v>67379</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>CONSOLIDATED COS</t>
+          <t>WESTERN HEALTH PLANS</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>JAC</t>
+          <t>WHP</t>
         </is>
       </c>
       <c r="D11" s="2" t="n">
         <v>31778</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>32574</v>
+        <v>32763</v>
       </c>
       <c r="F11" t="n">
         <v>2</v>
@@ -746,23 +746,23 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>67379</v>
+        <v>72098</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>WESTERN HEALTH PLANS</t>
+          <t>ISI SYSTEMS INC</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>WHP</t>
+          <t>SYS</t>
         </is>
       </c>
       <c r="D12" s="2" t="n">
-        <v>31778</v>
+        <v>31793</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>32763</v>
+        <v>32833</v>
       </c>
       <c r="F12" t="n">
         <v>2</v>
@@ -773,23 +773,23 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>72098</v>
+        <v>72581</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ISI SYSTEMS INC</t>
+          <t>RIVERBEND INTL CORP</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>SYS</t>
+          <t>RIV</t>
         </is>
       </c>
       <c r="D13" s="2" t="n">
-        <v>31793</v>
+        <v>31841</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>32833</v>
+        <v>33435</v>
       </c>
       <c r="F13" t="n">
         <v>2</v>
@@ -800,23 +800,23 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>72581</v>
+        <v>75079</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>RIVERBEND INTL CORP</t>
+          <t>NASTA INTERNATIONAL INC</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>RIV</t>
+          <t>NAS</t>
         </is>
       </c>
       <c r="D14" s="2" t="n">
-        <v>31841</v>
+        <v>31932</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>33435</v>
+        <v>33149</v>
       </c>
       <c r="F14" t="n">
         <v>2</v>
@@ -827,23 +827,23 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>75079</v>
+        <v>75090</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>NASTA INTERNATIONAL INC</t>
+          <t>ENSR CORP</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>NAS</t>
+          <t>RSE</t>
         </is>
       </c>
       <c r="D15" s="2" t="n">
-        <v>31932</v>
+        <v>31933</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>33149</v>
+        <v>33009</v>
       </c>
       <c r="F15" t="n">
         <v>2</v>
@@ -854,23 +854,23 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>75079</v>
+        <v>75048</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>NASTA INTERNATIONAL INC</t>
+          <t>COLORADO PRIME CORP</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>NAS</t>
+          <t>CPE</t>
         </is>
       </c>
       <c r="D16" s="2" t="n">
-        <v>31932</v>
+        <v>31953</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>33149</v>
+        <v>32771</v>
       </c>
       <c r="F16" t="n">
         <v>2</v>
@@ -881,50 +881,50 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>75090</v>
+        <v>75156</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ENSR CORP</t>
+          <t>CONTINENTAL GRAPHICS CORP</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>RSE</t>
+          <t>CIG</t>
         </is>
       </c>
       <c r="D17" s="2" t="n">
-        <v>31933</v>
+        <v>31988</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>33009</v>
+        <v>32448</v>
       </c>
       <c r="F17" t="n">
         <v>2</v>
       </c>
       <c r="G17" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>75048</v>
+        <v>75431</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>COLORADO PRIME CORP</t>
+          <t>WESTAIR HOLDING INC</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>CPE</t>
+          <t>WAH</t>
         </is>
       </c>
       <c r="D18" s="2" t="n">
-        <v>31953</v>
+        <v>32441</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>32771</v>
+        <v>33753</v>
       </c>
       <c r="F18" t="n">
         <v>2</v>
@@ -935,50 +935,50 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>75156</v>
+        <v>76186</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>CONTINENTAL GRAPHICS CORP</t>
+          <t>CHILES OFFSHORE CORP</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>CIG</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="D19" s="2" t="n">
-        <v>31988</v>
+        <v>33017</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>32448</v>
+        <v>34592</v>
       </c>
       <c r="F19" t="n">
         <v>2</v>
       </c>
       <c r="G19" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>75431</v>
+        <v>76097</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>WESTAIR HOLDING INC</t>
+          <t>CII FINANCIAL INC</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>WAH</t>
+          <t>CII</t>
         </is>
       </c>
       <c r="D20" s="2" t="n">
-        <v>32441</v>
+        <v>33221</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>33753</v>
+        <v>35002</v>
       </c>
       <c r="F20" t="n">
         <v>2</v>
@@ -989,23 +989,23 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>76186</v>
+        <v>10872</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>CHILES OFFSHORE CORP</t>
+          <t>FARRAGUT MORTGAGE CO INC</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>FMS</t>
         </is>
       </c>
       <c r="D21" s="2" t="n">
-        <v>33017</v>
+        <v>33659</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>34592</v>
+        <v>34470</v>
       </c>
       <c r="F21" t="n">
         <v>2</v>
@@ -1016,23 +1016,23 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>76097</v>
+        <v>77821</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>CII FINANCIAL INC</t>
+          <t>RHI ENTERTAINMENT INC-OLD</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>CII</t>
+          <t>RHE</t>
         </is>
       </c>
       <c r="D22" s="2" t="n">
-        <v>33221</v>
+        <v>33821</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>35002</v>
+        <v>34521</v>
       </c>
       <c r="F22" t="n">
         <v>2</v>
@@ -1043,23 +1043,23 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>10872</v>
+        <v>70893</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>FARRAGUT MORTGAGE CO INC</t>
+          <t>NEW LINE CINEMA CORP</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>FMS</t>
+          <t>NLN</t>
         </is>
       </c>
       <c r="D23" s="2" t="n">
-        <v>33659</v>
+        <v>34026</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>34470</v>
+        <v>34361</v>
       </c>
       <c r="F23" t="n">
         <v>2</v>
@@ -1070,23 +1070,23 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>77821</v>
+        <v>79757</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>RHI ENTERTAINMENT INC-OLD</t>
+          <t>APROGENEX INC</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>RHE</t>
+          <t>APG</t>
         </is>
       </c>
       <c r="D24" s="2" t="n">
-        <v>33821</v>
+        <v>34257</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>34521</v>
+        <v>35591</v>
       </c>
       <c r="F24" t="n">
         <v>2</v>
@@ -1097,23 +1097,23 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>70893</v>
+        <v>79772</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>NEW LINE CINEMA CORP</t>
+          <t>TRI-LITE INC</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>NLN</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="D25" s="2" t="n">
-        <v>34026</v>
+        <v>34262</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>34361</v>
+        <v>35093</v>
       </c>
       <c r="F25" t="n">
         <v>2</v>
@@ -1124,23 +1124,23 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>79757</v>
+        <v>80396</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>APROGENEX INC</t>
+          <t>JALATE LTD</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>APG</t>
+          <t>JLT</t>
         </is>
       </c>
       <c r="D26" s="2" t="n">
-        <v>34257</v>
+        <v>34409</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>35591</v>
+        <v>36160</v>
       </c>
       <c r="F26" t="n">
         <v>2</v>
@@ -1151,23 +1151,23 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>79772</v>
+        <v>80781</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>TRI-LITE INC</t>
+          <t>DIMAC CORP</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>DMC</t>
         </is>
       </c>
       <c r="D27" s="2" t="n">
-        <v>34262</v>
+        <v>34549</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>35093</v>
+        <v>35116</v>
       </c>
       <c r="F27" t="n">
         <v>2</v>
@@ -1178,23 +1178,23 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>79772</v>
+        <v>80788</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>TRI-LITE INC</t>
+          <t>SILVERADO FOODS INC</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>SLV</t>
         </is>
       </c>
       <c r="D28" s="2" t="n">
-        <v>34262</v>
+        <v>34550</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>35093</v>
+        <v>36140</v>
       </c>
       <c r="F28" t="n">
         <v>2</v>
@@ -1205,77 +1205,77 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>80396</v>
+        <v>81529</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>JALATE LTD</t>
+          <t>OMNI MULTIMEDIA GROUP INC</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>JLT</t>
+          <t>OMG</t>
         </is>
       </c>
       <c r="D29" s="2" t="n">
-        <v>34409</v>
+        <v>34809</v>
       </c>
       <c r="E29" s="2" t="n">
-        <v>36160</v>
+        <v>35748</v>
       </c>
       <c r="F29" t="n">
         <v>2</v>
       </c>
       <c r="G29" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>80781</v>
+        <v>82306</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>DIMAC CORP</t>
+          <t>STERLING HOUSE CORP</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>DMC</t>
+          <t>SGH</t>
         </is>
       </c>
       <c r="D30" s="2" t="n">
-        <v>34549</v>
+        <v>34998</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>35116</v>
+        <v>35726</v>
       </c>
       <c r="F30" t="n">
         <v>2</v>
       </c>
       <c r="G30" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>80788</v>
+        <v>82781</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>SILVERADO FOODS INC</t>
+          <t>PIEDMONT BANCORP INC</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>SLV</t>
+          <t>PDB</t>
         </is>
       </c>
       <c r="D31" s="2" t="n">
-        <v>34550</v>
+        <v>35042</v>
       </c>
       <c r="E31" s="2" t="n">
-        <v>36140</v>
+        <v>36627</v>
       </c>
       <c r="F31" t="n">
         <v>2</v>
@@ -1286,77 +1286,77 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>81529</v>
+        <v>83231</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>OMNI MULTIMEDIA GROUP INC</t>
+          <t>THERMOQUEST CORP</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>OMG</t>
+          <t>TMQ</t>
         </is>
       </c>
       <c r="D32" s="2" t="n">
-        <v>34809</v>
+        <v>35143</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>35748</v>
+        <v>36657</v>
       </c>
       <c r="F32" t="n">
         <v>2</v>
       </c>
       <c r="G32" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>82306</v>
+        <v>83230</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>STERLING HOUSE CORP</t>
+          <t>THERMO SENTRON INC</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>SGH</t>
+          <t>TSR</t>
         </is>
       </c>
       <c r="D33" s="2" t="n">
-        <v>34998</v>
+        <v>35151</v>
       </c>
       <c r="E33" s="2" t="n">
-        <v>35726</v>
+        <v>36615</v>
       </c>
       <c r="F33" t="n">
         <v>2</v>
       </c>
       <c r="G33" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>82781</v>
+        <v>83612</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>PIEDMONT BANCORP INC</t>
+          <t>THERMO OPTEK CORP</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>PDB</t>
+          <t>TOC</t>
         </is>
       </c>
       <c r="D34" s="2" t="n">
-        <v>35042</v>
+        <v>35223</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>36627</v>
+        <v>36657</v>
       </c>
       <c r="F34" t="n">
         <v>2</v>
@@ -1367,23 +1367,23 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>83231</v>
+        <v>83825</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>THERMOQUEST CORP</t>
+          <t>MIDCOAST ENERGY RES INC</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>TMQ</t>
+          <t>MRS</t>
         </is>
       </c>
       <c r="D35" s="2" t="n">
-        <v>35143</v>
+        <v>35286</v>
       </c>
       <c r="E35" s="2" t="n">
-        <v>36657</v>
+        <v>37022</v>
       </c>
       <c r="F35" t="n">
         <v>2</v>
@@ -1394,23 +1394,23 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>83230</v>
+        <v>84000</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>THERMO SENTRON INC</t>
+          <t>THERMO BIOANALYSIS CORP</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>TSR</t>
+          <t>TBA</t>
         </is>
       </c>
       <c r="D36" s="2" t="n">
-        <v>35151</v>
+        <v>35326</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>36615</v>
+        <v>36635</v>
       </c>
       <c r="F36" t="n">
         <v>2</v>
@@ -1421,23 +1421,23 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>83612</v>
+        <v>83990</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>THERMO OPTEK CORP</t>
+          <t>HALTER MARINE GROUP INC</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>TOC</t>
+          <t>HLX</t>
         </is>
       </c>
       <c r="D37" s="2" t="n">
-        <v>35223</v>
+        <v>35339</v>
       </c>
       <c r="E37" s="2" t="n">
-        <v>36657</v>
+        <v>36467</v>
       </c>
       <c r="F37" t="n">
         <v>2</v>
@@ -1448,23 +1448,23 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>83825</v>
+        <v>84583</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>MIDCOAST ENERGY RES INC</t>
+          <t>PURO WATER GROUP INC</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>MRS</t>
+          <t>HHO</t>
         </is>
       </c>
       <c r="D38" s="2" t="n">
-        <v>35286</v>
+        <v>35468</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>37022</v>
+        <v>35794</v>
       </c>
       <c r="F38" t="n">
         <v>2</v>
@@ -1475,23 +1475,23 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>84000</v>
+        <v>85069</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>THERMO BIOANALYSIS CORP</t>
+          <t>METRIKA SYSTEMS CORP</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>TBA</t>
+          <t>MKA</t>
         </is>
       </c>
       <c r="D39" s="2" t="n">
-        <v>35326</v>
+        <v>35604</v>
       </c>
       <c r="E39" s="2" t="n">
-        <v>36635</v>
+        <v>36648</v>
       </c>
       <c r="F39" t="n">
         <v>2</v>
@@ -1502,23 +1502,23 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>83990</v>
+        <v>85241</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>HALTER MARINE GROUP INC</t>
+          <t>HOME SECURITY INTL INC</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>HLX</t>
+          <t>HSI</t>
         </is>
       </c>
       <c r="D40" s="2" t="n">
-        <v>35339</v>
+        <v>35627</v>
       </c>
       <c r="E40" s="2" t="n">
-        <v>36467</v>
+        <v>37029</v>
       </c>
       <c r="F40" t="n">
         <v>2</v>
@@ -1529,23 +1529,23 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>84583</v>
+        <v>85258</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>PURO WATER GROUP INC</t>
+          <t>CLEARVIEW CINEMA GROUP INC</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>HHO</t>
+          <t>CLV</t>
         </is>
       </c>
       <c r="D41" s="2" t="n">
-        <v>35468</v>
+        <v>35661</v>
       </c>
       <c r="E41" s="2" t="n">
-        <v>35794</v>
+        <v>36131</v>
       </c>
       <c r="F41" t="n">
         <v>2</v>
@@ -1556,23 +1556,23 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>85069</v>
+        <v>85417</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>METRIKA SYSTEMS CORP</t>
+          <t>BIBB CO/DEL</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>MKA</t>
+          <t>BIB</t>
         </is>
       </c>
       <c r="D42" s="2" t="n">
-        <v>35604</v>
+        <v>35706</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>36648</v>
+        <v>36081</v>
       </c>
       <c r="F42" t="n">
         <v>2</v>
@@ -1583,23 +1583,23 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>85241</v>
+        <v>85598</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>HOME SECURITY INTL INC</t>
+          <t>BAYARD DRILLING TECHNOLOGIES</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>HSI</t>
+          <t>BDI</t>
         </is>
       </c>
       <c r="D43" s="2" t="n">
-        <v>35627</v>
+        <v>35738</v>
       </c>
       <c r="E43" s="2" t="n">
-        <v>37029</v>
+        <v>36257</v>
       </c>
       <c r="F43" t="n">
         <v>2</v>
@@ -1610,23 +1610,23 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>85258</v>
+        <v>85649</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>CLEARVIEW CINEMA GROUP INC</t>
+          <t>EQUALITY BANCORP INC</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>CLV</t>
+          <t>EBI</t>
         </is>
       </c>
       <c r="D44" s="2" t="n">
-        <v>35661</v>
+        <v>35766</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>36131</v>
+        <v>36845</v>
       </c>
       <c r="F44" t="n">
         <v>2</v>
@@ -1637,23 +1637,23 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>85417</v>
+        <v>85662</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>BIBB CO/DEL</t>
+          <t>THERMO VISION CORP</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>BIB</t>
+          <t>VIZ</t>
         </is>
       </c>
       <c r="D45" s="2" t="n">
-        <v>35706</v>
+        <v>35775</v>
       </c>
       <c r="E45" s="2" t="n">
-        <v>36081</v>
+        <v>36531</v>
       </c>
       <c r="F45" t="n">
         <v>2</v>
@@ -1664,23 +1664,23 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>85598</v>
+        <v>85648</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>BAYARD DRILLING TECHNOLOGIES</t>
+          <t>EMERGING COMMUNICATIONS INC</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>BDI</t>
+          <t>ECM</t>
         </is>
       </c>
       <c r="D46" s="2" t="n">
-        <v>35738</v>
+        <v>35795</v>
       </c>
       <c r="E46" s="2" t="n">
-        <v>36257</v>
+        <v>36068</v>
       </c>
       <c r="F46" t="n">
         <v>2</v>
@@ -1691,23 +1691,23 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>85649</v>
+        <v>85775</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>EQUALITY BANCORP INC</t>
+          <t>STANDARD AUTOMOTIVE CORP</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>EBI</t>
+          <t>AJX</t>
         </is>
       </c>
       <c r="D47" s="2" t="n">
-        <v>35766</v>
+        <v>35817</v>
       </c>
       <c r="E47" s="2" t="n">
-        <v>36845</v>
+        <v>37334</v>
       </c>
       <c r="F47" t="n">
         <v>2</v>
@@ -1718,23 +1718,23 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>85662</v>
+        <v>85782</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>THERMO VISION CORP</t>
+          <t>BALANCED CARE CORP</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>VIZ</t>
+          <t>BAL</t>
         </is>
       </c>
       <c r="D48" s="2" t="n">
-        <v>35775</v>
+        <v>35838</v>
       </c>
       <c r="E48" s="2" t="n">
-        <v>36531</v>
+        <v>37487</v>
       </c>
       <c r="F48" t="n">
         <v>2</v>
@@ -1745,23 +1745,23 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>85648</v>
+        <v>85787</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>EMERGING COMMUNICATIONS INC</t>
+          <t>ENVIRONMENTAL SAFEGUARDS INC</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>ECM</t>
+          <t>EVV</t>
         </is>
       </c>
       <c r="D49" s="2" t="n">
-        <v>35795</v>
+        <v>35839</v>
       </c>
       <c r="E49" s="2" t="n">
-        <v>36068</v>
+        <v>37544</v>
       </c>
       <c r="F49" t="n">
         <v>2</v>
@@ -1772,23 +1772,23 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>85775</v>
+        <v>85791</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>STANDARD AUTOMOTIVE CORP</t>
+          <t>GENEVA FINANCIAL CORP</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>AJX</t>
+          <t>PFC</t>
         </is>
       </c>
       <c r="D50" s="2" t="n">
-        <v>35817</v>
+        <v>35845</v>
       </c>
       <c r="E50" s="2" t="n">
-        <v>37334</v>
+        <v>36515</v>
       </c>
       <c r="F50" t="n">
         <v>2</v>
@@ -1799,23 +1799,23 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>85782</v>
+        <v>85927</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>BALANCED CARE CORP</t>
+          <t>SECURITY ASSOC INTL INC</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>BAL</t>
+          <t>IDL</t>
         </is>
       </c>
       <c r="D51" s="2" t="n">
-        <v>35838</v>
+        <v>35860</v>
       </c>
       <c r="E51" s="2" t="n">
-        <v>37487</v>
+        <v>37602</v>
       </c>
       <c r="F51" t="n">
         <v>2</v>
@@ -1826,23 +1826,23 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>85787</v>
+        <v>85901</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>ENVIRONMENTAL SAFEGUARDS INC</t>
+          <t>CPS SYSTEMS INC</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>EVV</t>
+          <t>SYS</t>
         </is>
       </c>
       <c r="D52" s="2" t="n">
-        <v>35839</v>
+        <v>35879</v>
       </c>
       <c r="E52" s="2" t="n">
-        <v>37544</v>
+        <v>36517</v>
       </c>
       <c r="F52" t="n">
         <v>2</v>
@@ -1853,23 +1853,23 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>85791</v>
+        <v>85919</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>GENEVA FINANCIAL CORP</t>
+          <t>ONIX SYSTEMS INC</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>PFC</t>
+          <t>ONX</t>
         </is>
       </c>
       <c r="D53" s="2" t="n">
-        <v>35845</v>
+        <v>35879</v>
       </c>
       <c r="E53" s="2" t="n">
-        <v>36515</v>
+        <v>36628</v>
       </c>
       <c r="F53" t="n">
         <v>2</v>
@@ -1880,23 +1880,23 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>85927</v>
+        <v>85928</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>SECURITY ASSOC INTL INC</t>
+          <t>SERACARE INC</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>IDL</t>
+          <t>SRK</t>
         </is>
       </c>
       <c r="D54" s="2" t="n">
-        <v>35860</v>
+        <v>35879</v>
       </c>
       <c r="E54" s="2" t="n">
-        <v>37602</v>
+        <v>37158</v>
       </c>
       <c r="F54" t="n">
         <v>2</v>
@@ -1907,23 +1907,23 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>85901</v>
+        <v>85936</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>CPS SYSTEMS INC</t>
+          <t>BLC FINANCIAL SERVICES INC</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>SYS</t>
+          <t>BCL</t>
         </is>
       </c>
       <c r="D55" s="2" t="n">
-        <v>35879</v>
+        <v>35916</v>
       </c>
       <c r="E55" s="2" t="n">
-        <v>36517</v>
+        <v>36889</v>
       </c>
       <c r="F55" t="n">
         <v>2</v>
@@ -1934,23 +1934,23 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>85919</v>
+        <v>86137</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>ONIX SYSTEMS INC</t>
+          <t>SHOWPOWER INC</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>ONX</t>
+          <t>SHO</t>
         </is>
       </c>
       <c r="D56" s="2" t="n">
-        <v>35879</v>
+        <v>35962</v>
       </c>
       <c r="E56" s="2" t="n">
-        <v>36628</v>
+        <v>36553</v>
       </c>
       <c r="F56" t="n">
         <v>2</v>
@@ -1961,23 +1961,23 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>85928</v>
+        <v>86344</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>SERACARE INC</t>
+          <t>EASYRIDERS INC</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>SRK</t>
+          <t>EZR</t>
         </is>
       </c>
       <c r="D57" s="2" t="n">
-        <v>35879</v>
+        <v>36062</v>
       </c>
       <c r="E57" s="2" t="n">
-        <v>37158</v>
+        <v>37089</v>
       </c>
       <c r="F57" t="n">
         <v>2</v>
@@ -1988,23 +1988,23 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>85936</v>
+        <v>86379</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>BLC FINANCIAL SERVICES INC</t>
+          <t>VORNADO OPERATING CO</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>BCL</t>
+          <t>VOO</t>
         </is>
       </c>
       <c r="D58" s="2" t="n">
-        <v>35916</v>
+        <v>36084</v>
       </c>
       <c r="E58" s="2" t="n">
-        <v>36889</v>
+        <v>37813</v>
       </c>
       <c r="F58" t="n">
         <v>2</v>
@@ -2015,23 +2015,23 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>86137</v>
+        <v>86446</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>SHOWPOWER INC</t>
+          <t>JCC HOLDING CO</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>SHO</t>
+          <t>JAZ</t>
         </is>
       </c>
       <c r="D59" s="2" t="n">
-        <v>35962</v>
+        <v>36138</v>
       </c>
       <c r="E59" s="2" t="n">
-        <v>36553</v>
+        <v>36859</v>
       </c>
       <c r="F59" t="n">
         <v>2</v>
@@ -2042,23 +2042,23 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>86344</v>
+        <v>86459</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>EASYRIDERS INC</t>
+          <t>SECURITY PA FINANCIAL CORP</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>EZR</t>
+          <t>SPN</t>
         </is>
       </c>
       <c r="D60" s="2" t="n">
-        <v>36062</v>
+        <v>36159</v>
       </c>
       <c r="E60" s="2" t="n">
-        <v>37089</v>
+        <v>36840</v>
       </c>
       <c r="F60" t="n">
         <v>2</v>
@@ -2069,23 +2069,23 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>86379</v>
+        <v>86940</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>VORNADO OPERATING CO</t>
+          <t>C-3D DIGITAL INC</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>VOO</t>
+          <t>DDD</t>
         </is>
       </c>
       <c r="D61" s="2" t="n">
-        <v>36084</v>
+        <v>36320</v>
       </c>
       <c r="E61" s="2" t="n">
-        <v>37813</v>
+        <v>37586</v>
       </c>
       <c r="F61" t="n">
         <v>2</v>
@@ -2096,23 +2096,23 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>86446</v>
+        <v>87028</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>JCC HOLDING CO</t>
+          <t>CARESIDE INC</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>JAZ</t>
+          <t>CSA</t>
         </is>
       </c>
       <c r="D62" s="2" t="n">
-        <v>36138</v>
+        <v>36360</v>
       </c>
       <c r="E62" s="2" t="n">
-        <v>36859</v>
+        <v>37546</v>
       </c>
       <c r="F62" t="n">
         <v>2</v>
@@ -2123,23 +2123,23 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>86459</v>
+        <v>87216</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>SECURITY PA FINANCIAL CORP</t>
+          <t>ENVISION DEVELOPMENT CORP</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>SPN</t>
+          <t>PF</t>
         </is>
       </c>
       <c r="D63" s="2" t="n">
-        <v>36159</v>
+        <v>36432</v>
       </c>
       <c r="E63" s="2" t="n">
-        <v>36840</v>
+        <v>36833</v>
       </c>
       <c r="F63" t="n">
         <v>2</v>
@@ -2150,23 +2150,23 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>86940</v>
+        <v>87287</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>C-3D DIGITAL INC</t>
+          <t>RAMPART CAPITAL CORP</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>DDD</t>
+          <t>RAC</t>
         </is>
       </c>
       <c r="D64" s="2" t="n">
-        <v>36320</v>
+        <v>36455</v>
       </c>
       <c r="E64" s="2" t="n">
-        <v>37586</v>
+        <v>37930</v>
       </c>
       <c r="F64" t="n">
         <v>2</v>
@@ -2177,23 +2177,23 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>87028</v>
+        <v>87468</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>CARESIDE INC</t>
+          <t>PLASTIC SURGERY CO</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>CSA</t>
+          <t>PSU</t>
         </is>
       </c>
       <c r="D65" s="2" t="n">
-        <v>36360</v>
+        <v>36504</v>
       </c>
       <c r="E65" s="2" t="n">
-        <v>37546</v>
+        <v>37343</v>
       </c>
       <c r="F65" t="n">
         <v>2</v>
@@ -2204,23 +2204,23 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>87216</v>
+        <v>87470</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>ENVISION DEVELOPMENT CORP</t>
+          <t>PREMIER BANCORP INC/PA</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>PF</t>
+          <t>PPA</t>
         </is>
       </c>
       <c r="D66" s="2" t="n">
-        <v>36432</v>
+        <v>36524</v>
       </c>
       <c r="E66" s="2" t="n">
-        <v>36833</v>
+        <v>37833</v>
       </c>
       <c r="F66" t="n">
         <v>2</v>
@@ -2231,23 +2231,23 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>87287</v>
+        <v>87663</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>RAMPART CAPITAL CORP</t>
+          <t>IMPERIAL PARKING CORP</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>RAC</t>
+          <t>IPK</t>
         </is>
       </c>
       <c r="D67" s="2" t="n">
-        <v>36455</v>
+        <v>36613</v>
       </c>
       <c r="E67" s="2" t="n">
-        <v>37930</v>
+        <v>38111</v>
       </c>
       <c r="F67" t="n">
         <v>2</v>
@@ -2258,23 +2258,23 @@
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>87468</v>
+        <v>87836</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>PLASTIC SURGERY CO</t>
+          <t>FIRST CITY BK NEW BRITIAN CO</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>PSU</t>
+          <t>FBK</t>
         </is>
       </c>
       <c r="D68" s="2" t="n">
-        <v>36504</v>
+        <v>36641</v>
       </c>
       <c r="E68" s="2" t="n">
-        <v>37343</v>
+        <v>38324</v>
       </c>
       <c r="F68" t="n">
         <v>2</v>
@@ -2285,23 +2285,23 @@
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>87470</v>
+        <v>88316</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>PREMIER BANCORP INC/PA</t>
+          <t>TELZUIT MEDICAL TECH INC</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>PPA</t>
+          <t>TTA</t>
         </is>
       </c>
       <c r="D69" s="2" t="n">
-        <v>36524</v>
+        <v>36690</v>
       </c>
       <c r="E69" s="2" t="n">
-        <v>37833</v>
+        <v>38142</v>
       </c>
       <c r="F69" t="n">
         <v>2</v>
@@ -2312,23 +2312,23 @@
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>87663</v>
+        <v>88288</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>IMPERIAL PARKING CORP</t>
+          <t>DUCK HEAD APPAREL CO INC</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>IPK</t>
+          <t>DHA</t>
         </is>
       </c>
       <c r="D70" s="2" t="n">
-        <v>36613</v>
+        <v>36707</v>
       </c>
       <c r="E70" s="2" t="n">
-        <v>38111</v>
+        <v>37112</v>
       </c>
       <c r="F70" t="n">
         <v>2</v>
@@ -2339,23 +2339,23 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>87836</v>
+        <v>88588</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>FIRST CITY BK NEW BRITIAN CO</t>
+          <t>CHILES OFFSHORE INC</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>FBK</t>
+          <t>COD</t>
         </is>
       </c>
       <c r="D71" s="2" t="n">
-        <v>36641</v>
+        <v>36788</v>
       </c>
       <c r="E71" s="2" t="n">
-        <v>38324</v>
+        <v>37475</v>
       </c>
       <c r="F71" t="n">
         <v>2</v>
@@ -2366,23 +2366,23 @@
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>88316</v>
+        <v>88886</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>TELZUIT MEDICAL TECH INC</t>
+          <t>AQUACELL TECHNOLOGIES INC</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>TTA</t>
+          <t>AQA</t>
         </is>
       </c>
       <c r="D72" s="2" t="n">
-        <v>36690</v>
+        <v>36934</v>
       </c>
       <c r="E72" s="2" t="n">
-        <v>38142</v>
+        <v>38709</v>
       </c>
       <c r="F72" t="n">
         <v>2</v>
@@ -2393,23 +2393,23 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>88288</v>
+        <v>89328</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>DUCK HEAD APPAREL CO INC</t>
+          <t>CAP ROCK ENERGY CORP</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>DHA</t>
+          <t>RKE</t>
         </is>
       </c>
       <c r="D73" s="2" t="n">
-        <v>36707</v>
+        <v>37329</v>
       </c>
       <c r="E73" s="2" t="n">
-        <v>37112</v>
+        <v>38848</v>
       </c>
       <c r="F73" t="n">
         <v>2</v>
@@ -2420,23 +2420,23 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>88588</v>
+        <v>89434</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>CHILES OFFSHORE INC</t>
+          <t>MONTANA MILLS BREAD CO</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>COD</t>
+          <t>MMX</t>
         </is>
       </c>
       <c r="D74" s="2" t="n">
-        <v>36788</v>
+        <v>37435</v>
       </c>
       <c r="E74" s="2" t="n">
-        <v>37475</v>
+        <v>37718</v>
       </c>
       <c r="F74" t="n">
         <v>2</v>
@@ -2447,23 +2447,23 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>88886</v>
+        <v>89963</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>AQUACELL TECHNOLOGIES INC</t>
+          <t>NATURAL GOLF CORP</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>AQA</t>
+          <t>NAX</t>
         </is>
       </c>
       <c r="D75" s="2" t="n">
-        <v>36934</v>
+        <v>37967</v>
       </c>
       <c r="E75" s="2" t="n">
-        <v>38709</v>
+        <v>38457</v>
       </c>
       <c r="F75" t="n">
         <v>2</v>
@@ -2474,23 +2474,23 @@
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>89328</v>
+        <v>90311</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>CAP ROCK ENERGY CORP</t>
+          <t>SAMARITAN PHARMACEUTICALS</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>RKE</t>
+          <t>LIV</t>
         </is>
       </c>
       <c r="D76" s="2" t="n">
-        <v>37329</v>
+        <v>38225</v>
       </c>
       <c r="E76" s="2" t="n">
-        <v>38848</v>
+        <v>39430</v>
       </c>
       <c r="F76" t="n">
         <v>2</v>
@@ -2501,23 +2501,23 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>89434</v>
+        <v>90341</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>MONTANA MILLS BREAD CO</t>
+          <t>NEPHROS INC</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>MMX</t>
+          <t>NEP</t>
         </is>
       </c>
       <c r="D77" s="2" t="n">
-        <v>37435</v>
+        <v>38251</v>
       </c>
       <c r="E77" s="2" t="n">
-        <v>37718</v>
+        <v>39834</v>
       </c>
       <c r="F77" t="n">
         <v>2</v>
@@ -2528,23 +2528,23 @@
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>89963</v>
+        <v>90566</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>NATURAL GOLF CORP</t>
+          <t>TARPON INDUSTRIES INC</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>NAX</t>
+          <t>TPO</t>
         </is>
       </c>
       <c r="D78" s="2" t="n">
-        <v>37967</v>
+        <v>38397</v>
       </c>
       <c r="E78" s="2" t="n">
-        <v>38457</v>
+        <v>39399</v>
       </c>
       <c r="F78" t="n">
         <v>2</v>
@@ -2555,23 +2555,23 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>90311</v>
+        <v>90653</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>SAMARITAN PHARMACEUTICALS</t>
+          <t>BLACK RAVEN ENERGY INC</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>LIV</t>
+          <t>PRB</t>
         </is>
       </c>
       <c r="D79" s="2" t="n">
-        <v>38225</v>
+        <v>38454</v>
       </c>
       <c r="E79" s="2" t="n">
-        <v>39430</v>
+        <v>39513</v>
       </c>
       <c r="F79" t="n">
         <v>2</v>
@@ -2582,23 +2582,23 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>90341</v>
+        <v>90759</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>NEPHROS INC</t>
+          <t>HEMOSENSE INC</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>NEP</t>
+          <t>HEM</t>
         </is>
       </c>
       <c r="D80" s="2" t="n">
-        <v>38251</v>
+        <v>38531</v>
       </c>
       <c r="E80" s="2" t="n">
-        <v>39834</v>
+        <v>39392</v>
       </c>
       <c r="F80" t="n">
         <v>2</v>
@@ -2609,23 +2609,23 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>90566</v>
+        <v>90830</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>TARPON INDUSTRIES INC</t>
+          <t>AMERICAN COMMUNITY NEWSPAPER</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>TPO</t>
+          <t>CRB</t>
         </is>
       </c>
       <c r="D81" s="2" t="n">
-        <v>38397</v>
+        <v>38566</v>
       </c>
       <c r="E81" s="2" t="n">
-        <v>39399</v>
+        <v>39759</v>
       </c>
       <c r="F81" t="n">
         <v>2</v>
@@ -2636,23 +2636,23 @@
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>90653</v>
+        <v>91042</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>BLACK RAVEN ENERGY INC</t>
+          <t>COLD SPRING CAPITAL INC</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>PRB</t>
+          <t>CDS</t>
         </is>
       </c>
       <c r="D82" s="2" t="n">
-        <v>38454</v>
+        <v>38698</v>
       </c>
       <c r="E82" s="2" t="n">
-        <v>39513</v>
+        <v>39206</v>
       </c>
       <c r="F82" t="n">
         <v>2</v>
@@ -2663,23 +2663,23 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>90759</v>
+        <v>91105</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>HEMOSENSE INC</t>
+          <t>AMERICAN TELECOM SERVICES</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>HEM</t>
+          <t>TES</t>
         </is>
       </c>
       <c r="D83" s="2" t="n">
-        <v>38531</v>
+        <v>38749</v>
       </c>
       <c r="E83" s="2" t="n">
-        <v>39392</v>
+        <v>39406</v>
       </c>
       <c r="F83" t="n">
         <v>2</v>
@@ -2690,23 +2690,23 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>90830</v>
+        <v>91190</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>AMERICAN COMMUNITY NEWSPAPER</t>
+          <t>JAZZ TECHNOLOGIES INC</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>CRB</t>
+          <t>AQR</t>
         </is>
       </c>
       <c r="D84" s="2" t="n">
-        <v>38566</v>
+        <v>38811</v>
       </c>
       <c r="E84" s="2" t="n">
-        <v>39759</v>
+        <v>39709</v>
       </c>
       <c r="F84" t="n">
         <v>2</v>
@@ -2717,23 +2717,23 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>91042</v>
+        <v>91569</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>COLD SPRING CAPITAL INC</t>
+          <t>DEBT RESOLVE INC</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>CDS</t>
+          <t>DRV</t>
         </is>
       </c>
       <c r="D85" s="2" t="n">
-        <v>38698</v>
+        <v>39022</v>
       </c>
       <c r="E85" s="2" t="n">
-        <v>39206</v>
+        <v>39717</v>
       </c>
       <c r="F85" t="n">
         <v>2</v>
@@ -2744,23 +2744,23 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>91105</v>
+        <v>92112</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>AMERICAN TELECOM SERVICES</t>
+          <t>CHINA SHENGHUO PHARM HLDGS</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>TES</t>
+          <t>KUN</t>
         </is>
       </c>
       <c r="D86" s="2" t="n">
-        <v>38749</v>
+        <v>39247</v>
       </c>
       <c r="E86" s="2" t="n">
-        <v>39406</v>
+        <v>41038</v>
       </c>
       <c r="F86" t="n">
         <v>2</v>
@@ -2771,23 +2771,23 @@
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>91190</v>
+        <v>92256</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>JAZZ TECHNOLOGIES INC</t>
+          <t>TWIN VEE POWERCATS INC</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>AQR</t>
+          <t>IVA</t>
         </is>
       </c>
       <c r="D87" s="2" t="n">
-        <v>38811</v>
+        <v>39301</v>
       </c>
       <c r="E87" s="2" t="n">
-        <v>39709</v>
+        <v>40534</v>
       </c>
       <c r="F87" t="n">
         <v>2</v>
@@ -2798,23 +2798,23 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>91569</v>
+        <v>92235</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>DEBT RESOLVE INC</t>
+          <t>BROOKE CAPITAL CORP</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>DRV</t>
+          <t>BCP</t>
         </is>
       </c>
       <c r="D88" s="2" t="n">
-        <v>39022</v>
+        <v>39324</v>
       </c>
       <c r="E88" s="2" t="n">
-        <v>39717</v>
+        <v>39744</v>
       </c>
       <c r="F88" t="n">
         <v>2</v>
@@ -2825,23 +2825,23 @@
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>92112</v>
+        <v>92484</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>CHINA SHENGHUO PHARM HLDGS</t>
+          <t>GULFSTREAM INTL GROUP INC</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>KUN</t>
+          <t>GIA</t>
         </is>
       </c>
       <c r="D89" s="2" t="n">
-        <v>39247</v>
+        <v>39430</v>
       </c>
       <c r="E89" s="2" t="n">
-        <v>41038</v>
+        <v>40486</v>
       </c>
       <c r="F89" t="n">
         <v>2</v>
@@ -2852,23 +2852,23 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>92256</v>
+        <v>92645</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>TWIN VEE POWERCATS INC</t>
+          <t>AMERICAN DEFENSE SYSTEMS INC</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>IVA</t>
+          <t>EAG</t>
         </is>
       </c>
       <c r="D90" s="2" t="n">
-        <v>39301</v>
+        <v>39598</v>
       </c>
       <c r="E90" s="2" t="n">
-        <v>40534</v>
+        <v>40877</v>
       </c>
       <c r="F90" t="n">
         <v>2</v>
@@ -2879,23 +2879,23 @@
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>92235</v>
+        <v>92861</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>BROOKE CAPITAL CORP</t>
+          <t>HERALD NATIONAL BANK</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>BCP</t>
+          <t>HNB</t>
         </is>
       </c>
       <c r="D91" s="2" t="n">
-        <v>39324</v>
+        <v>39791</v>
       </c>
       <c r="E91" s="2" t="n">
-        <v>39744</v>
+        <v>40968</v>
       </c>
       <c r="F91" t="n">
         <v>2</v>
@@ -2906,23 +2906,23 @@
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>92484</v>
+        <v>92899</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>GULFSTREAM INTL GROUP INC</t>
+          <t>NIVS INTELLIMEDIA TECHNOLOGY</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>GIA</t>
+          <t>NIV</t>
         </is>
       </c>
       <c r="D92" s="2" t="n">
-        <v>39430</v>
+        <v>39885</v>
       </c>
       <c r="E92" s="2" t="n">
-        <v>40486</v>
+        <v>40626</v>
       </c>
       <c r="F92" t="n">
         <v>2</v>
@@ -2933,23 +2933,23 @@
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>92645</v>
+        <v>93405</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>AMERICAN DEFENSE SYSTEMS INC</t>
+          <t>CHINA INTELLIGENT LTG &amp; ELCT</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>EAG</t>
+          <t>CIL</t>
         </is>
       </c>
       <c r="D93" s="2" t="n">
-        <v>39598</v>
+        <v>40347</v>
       </c>
       <c r="E93" s="2" t="n">
-        <v>40877</v>
+        <v>40626</v>
       </c>
       <c r="F93" t="n">
         <v>2</v>
@@ -2960,23 +2960,23 @@
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>92861</v>
+        <v>12440</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>HERALD NATIONAL BANK</t>
+          <t>CTPARTNERS EXEC SEARCH INC</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>HNB</t>
+          <t>CTP</t>
         </is>
       </c>
       <c r="D94" s="2" t="n">
-        <v>39791</v>
+        <v>40520</v>
       </c>
       <c r="E94" s="2" t="n">
-        <v>40968</v>
+        <v>42177</v>
       </c>
       <c r="F94" t="n">
         <v>2</v>
@@ -2987,23 +2987,23 @@
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>92899</v>
+        <v>12544</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>NIVS INTELLIMEDIA TECHNOLOGY</t>
+          <t>CHINA CENTURY DRAGON MEDIA</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>NIV</t>
+          <t>CDM</t>
         </is>
       </c>
       <c r="D95" s="2" t="n">
-        <v>39885</v>
+        <v>40582</v>
       </c>
       <c r="E95" s="2" t="n">
-        <v>40626</v>
+        <v>40620</v>
       </c>
       <c r="F95" t="n">
         <v>2</v>
@@ -3014,23 +3014,23 @@
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>93405</v>
+        <v>14335</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>CHINA INTELLIGENT LTG &amp; ELCT</t>
+          <t>CHENIERE ENERGY PTNRS LP LLC</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>CIL</t>
+          <t>CQH</t>
         </is>
       </c>
       <c r="D96" s="2" t="n">
-        <v>40347</v>
+        <v>41621</v>
       </c>
       <c r="E96" s="2" t="n">
-        <v>40626</v>
+        <v>43362</v>
       </c>
       <c r="F96" t="n">
         <v>2</v>
@@ -3041,23 +3041,23 @@
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>12440</v>
+        <v>19515</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>CTPARTNERS EXEC SEARCH INC</t>
+          <t>POLISHED.COM INC</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>CTP</t>
+          <t>GOED</t>
         </is>
       </c>
       <c r="D97" s="2" t="n">
-        <v>40520</v>
+        <v>44043</v>
       </c>
       <c r="E97" s="2" t="n">
-        <v>42177</v>
+        <v>45351</v>
       </c>
       <c r="F97" t="n">
         <v>2</v>
@@ -3068,23 +3068,23 @@
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>12544</v>
+        <v>19778</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>CHINA CENTURY DRAGON MEDIA</t>
+          <t>LAIRD SUPERFOOD INC</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>CDM</t>
+          <t>LSF</t>
         </is>
       </c>
       <c r="D98" s="2" t="n">
-        <v>40582</v>
+        <v>44097</v>
       </c>
       <c r="E98" s="2" t="n">
-        <v>40620</v>
+        <v>45657</v>
       </c>
       <c r="F98" t="n">
         <v>2</v>
@@ -3095,23 +3095,23 @@
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>14335</v>
+        <v>21664</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>CHENIERE ENERGY PTNRS LP LLC</t>
+          <t>MOVING IMAGE TECHNOLOGIS INC</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>CQH</t>
+          <t>MITQ</t>
         </is>
       </c>
       <c r="D99" s="2" t="n">
-        <v>41621</v>
+        <v>44385</v>
       </c>
       <c r="E99" s="2" t="n">
-        <v>43362</v>
+        <v>45657</v>
       </c>
       <c r="F99" t="n">
         <v>2</v>
@@ -3122,23 +3122,23 @@
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>19515</v>
+        <v>19417</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>POLISHED.COM INC</t>
+          <t>RENOVACOR INC</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>GOED</t>
+          <t>RCOR</t>
         </is>
       </c>
       <c r="D100" s="2" t="n">
-        <v>44043</v>
+        <v>44442</v>
       </c>
       <c r="E100" s="2" t="n">
-        <v>45351</v>
+        <v>44895</v>
       </c>
       <c r="F100" t="n">
         <v>2</v>
@@ -3149,23 +3149,23 @@
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>19778</v>
+        <v>22417</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>LAIRD SUPERFOOD INC</t>
+          <t>WINC INC</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>LSF</t>
+          <t>WBEV</t>
         </is>
       </c>
       <c r="D101" s="2" t="n">
-        <v>44097</v>
+        <v>44511</v>
       </c>
       <c r="E101" s="2" t="n">
-        <v>45657</v>
+        <v>44907</v>
       </c>
       <c r="F101" t="n">
         <v>2</v>
@@ -3176,20 +3176,20 @@
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>21664</v>
+        <v>22465</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>MOVING IMAGE TECHNOLOGIS INC</t>
+          <t>AMAZE HOLDINGS INC</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>MITQ</t>
+          <t>VINE</t>
         </is>
       </c>
       <c r="D102" s="2" t="n">
-        <v>44385</v>
+        <v>44544</v>
       </c>
       <c r="E102" s="2" t="n">
         <v>45657</v>
@@ -3203,23 +3203,23 @@
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>19417</v>
+        <v>22995</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>RENOVACOR INC</t>
+          <t>DAKOTA GOLD CORP</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>RCOR</t>
+          <t>DC</t>
         </is>
       </c>
       <c r="D103" s="2" t="n">
-        <v>44442</v>
+        <v>44656</v>
       </c>
       <c r="E103" s="2" t="n">
-        <v>44895</v>
+        <v>45657</v>
       </c>
       <c r="F103" t="n">
         <v>2</v>
@@ -3230,23 +3230,23 @@
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>22417</v>
+        <v>23147</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>WINC INC</t>
+          <t>IVANHOE ELECTRIC INC</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>WBEV</t>
+          <t>IE</t>
         </is>
       </c>
       <c r="D104" s="2" t="n">
-        <v>44511</v>
+        <v>44740</v>
       </c>
       <c r="E104" s="2" t="n">
-        <v>44907</v>
+        <v>45657</v>
       </c>
       <c r="F104" t="n">
         <v>2</v>
@@ -3257,20 +3257,20 @@
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>22465</v>
+        <v>23216</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>AMAZE HOLDINGS INC</t>
+          <t>MAIA BIOTECHNOLOGY INC</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>VINE</t>
+          <t>MAIA</t>
         </is>
       </c>
       <c r="D105" s="2" t="n">
-        <v>44544</v>
+        <v>44770</v>
       </c>
       <c r="E105" s="2" t="n">
         <v>45657</v>
@@ -3284,20 +3284,20 @@
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>22995</v>
+        <v>23849</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>DAKOTA GOLD CORP</t>
+          <t>TRIO PETROLEUM CORP</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>DC</t>
+          <t>TPET</t>
         </is>
       </c>
       <c r="D106" s="2" t="n">
-        <v>44656</v>
+        <v>45034</v>
       </c>
       <c r="E106" s="2" t="n">
         <v>45657</v>
@@ -3311,20 +3311,20 @@
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>23147</v>
+        <v>23951</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>IVANHOE ELECTRIC INC</t>
+          <t>AZITRA INC</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>IE</t>
+          <t>AZTR</t>
         </is>
       </c>
       <c r="D107" s="2" t="n">
-        <v>44740</v>
+        <v>45093</v>
       </c>
       <c r="E107" s="2" t="n">
         <v>45657</v>
@@ -3338,20 +3338,20 @@
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>23216</v>
+        <v>24087</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>MAIA BIOTECHNOLOGY INC</t>
+          <t>NEURAXIS INC</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>MAIA</t>
+          <t>NRXS</t>
         </is>
       </c>
       <c r="D108" s="2" t="n">
-        <v>44770</v>
+        <v>45147</v>
       </c>
       <c r="E108" s="2" t="n">
         <v>45657</v>
@@ -3365,20 +3365,20 @@
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>23849</v>
+        <v>24435</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>TRIO PETROLEUM CORP</t>
+          <t>NORTHANN CORP</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>TPET</t>
+          <t>NCL</t>
         </is>
       </c>
       <c r="D109" s="2" t="n">
-        <v>45034</v>
+        <v>45218</v>
       </c>
       <c r="E109" s="2" t="n">
         <v>45657</v>
@@ -3392,20 +3392,20 @@
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>23951</v>
+        <v>24507</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>AZITRA INC</t>
+          <t>SIGNING DAY SPORTS INC</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>AZTR</t>
+          <t>SGN</t>
         </is>
       </c>
       <c r="D110" s="2" t="n">
-        <v>45093</v>
+        <v>45244</v>
       </c>
       <c r="E110" s="2" t="n">
         <v>45657</v>
@@ -3419,20 +3419,20 @@
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>24087</v>
+        <v>24813</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>NEURAXIS INC</t>
+          <t>PERFECT MOMENT LTD</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>NRXS</t>
+          <t>PMNT</t>
         </is>
       </c>
       <c r="D111" s="2" t="n">
-        <v>45147</v>
+        <v>45330</v>
       </c>
       <c r="E111" s="2" t="n">
         <v>45657</v>
@@ -3446,20 +3446,20 @@
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>24435</v>
+        <v>24815</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>NORTHANN CORP</t>
+          <t>UNUSUAL MACHINES INC</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>NCL</t>
+          <t>UMAC</t>
         </is>
       </c>
       <c r="D112" s="2" t="n">
-        <v>45218</v>
+        <v>45336</v>
       </c>
       <c r="E112" s="2" t="n">
         <v>45657</v>
@@ -3473,20 +3473,20 @@
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>24507</v>
+        <v>24810</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>SIGNING DAY SPORTS INC</t>
+          <t>PELTHOS THERAPEUTICS INC</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>SGN</t>
+          <t>CHRO</t>
         </is>
       </c>
       <c r="D113" s="2" t="n">
-        <v>45244</v>
+        <v>45338</v>
       </c>
       <c r="E113" s="2" t="n">
         <v>45657</v>
@@ -3500,20 +3500,20 @@
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>24813</v>
+        <v>24983</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>PERFECT MOMENT LTD</t>
+          <t>CLEANCORE SOLUTIONS INC</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>PMNT</t>
+          <t>ZONE</t>
         </is>
       </c>
       <c r="D114" s="2" t="n">
-        <v>45330</v>
+        <v>45408</v>
       </c>
       <c r="E114" s="2" t="n">
         <v>45657</v>
@@ -3527,20 +3527,20 @@
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>24815</v>
+        <v>25362</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>UNUSUAL MACHINES INC</t>
+          <t>OS THERAPIES INC</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>UMAC</t>
+          <t>OSTX</t>
         </is>
       </c>
       <c r="D115" s="2" t="n">
-        <v>45336</v>
+        <v>45505</v>
       </c>
       <c r="E115" s="2" t="n">
         <v>45657</v>
@@ -3554,20 +3554,20 @@
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>24810</v>
+        <v>25471</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>PELTHOS THERAPEUTICS INC</t>
+          <t>IMPACT BIOMEDICAL INC</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>CHRO</t>
+          <t>IBO</t>
         </is>
       </c>
       <c r="D116" s="2" t="n">
-        <v>45338</v>
+        <v>45551</v>
       </c>
       <c r="E116" s="2" t="n">
         <v>45657</v>
@@ -3581,20 +3581,20 @@
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>24983</v>
+        <v>25481</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>CLEANCORE SOLUTIONS INC</t>
+          <t>KAIROS PHARMA LTD</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>ZONE</t>
+          <t>KAPA</t>
         </is>
       </c>
       <c r="D117" s="2" t="n">
-        <v>45408</v>
+        <v>45551</v>
       </c>
       <c r="E117" s="2" t="n">
         <v>45657</v>
@@ -3608,20 +3608,20 @@
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>25362</v>
+        <v>25482</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>OS THERAPIES INC</t>
+          <t>LEGACY EDUCATION INC</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>OSTX</t>
+          <t>LGCY</t>
         </is>
       </c>
       <c r="D118" s="2" t="n">
-        <v>45505</v>
+        <v>45561</v>
       </c>
       <c r="E118" s="2" t="n">
         <v>45657</v>
@@ -3635,20 +3635,20 @@
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>25471</v>
+        <v>25684</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>IMPACT BIOMEDICAL INC</t>
+          <t>HIGH ROLLER TECHNOLOGIES INC</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>IBO</t>
+          <t>ROLR</t>
         </is>
       </c>
       <c r="D119" s="2" t="n">
-        <v>45551</v>
+        <v>45588</v>
       </c>
       <c r="E119" s="2" t="n">
         <v>45657</v>
@@ -3662,20 +3662,20 @@
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>25481</v>
+        <v>25829</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>KAIROS PHARMA LTD</t>
+          <t>VENU HOLDING CORP</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>KAPA</t>
+          <t>VENU</t>
         </is>
       </c>
       <c r="D120" s="2" t="n">
-        <v>45551</v>
+        <v>45623</v>
       </c>
       <c r="E120" s="2" t="n">
         <v>45657</v>
@@ -3684,87 +3684,6 @@
         <v>2</v>
       </c>
       <c r="G120" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="n">
-        <v>25482</v>
-      </c>
-      <c r="B121" t="inlineStr">
-        <is>
-          <t>LEGACY EDUCATION INC</t>
-        </is>
-      </c>
-      <c r="C121" t="inlineStr">
-        <is>
-          <t>LGCY</t>
-        </is>
-      </c>
-      <c r="D121" s="2" t="n">
-        <v>45561</v>
-      </c>
-      <c r="E121" s="2" t="n">
-        <v>45657</v>
-      </c>
-      <c r="F121" t="n">
-        <v>2</v>
-      </c>
-      <c r="G121" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="n">
-        <v>25684</v>
-      </c>
-      <c r="B122" t="inlineStr">
-        <is>
-          <t>HIGH ROLLER TECHNOLOGIES INC</t>
-        </is>
-      </c>
-      <c r="C122" t="inlineStr">
-        <is>
-          <t>ROLR</t>
-        </is>
-      </c>
-      <c r="D122" s="2" t="n">
-        <v>45588</v>
-      </c>
-      <c r="E122" s="2" t="n">
-        <v>45657</v>
-      </c>
-      <c r="F122" t="n">
-        <v>2</v>
-      </c>
-      <c r="G122" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="n">
-        <v>25829</v>
-      </c>
-      <c r="B123" t="inlineStr">
-        <is>
-          <t>VENU HOLDING CORP</t>
-        </is>
-      </c>
-      <c r="C123" t="inlineStr">
-        <is>
-          <t>VENU</t>
-        </is>
-      </c>
-      <c r="D123" s="2" t="n">
-        <v>45623</v>
-      </c>
-      <c r="E123" s="2" t="n">
-        <v>45657</v>
-      </c>
-      <c r="F123" t="n">
-        <v>2</v>
-      </c>
-      <c r="G123" t="n">
         <v>11</v>
       </c>
     </row>

</xml_diff>